<commit_message>
Worked on making changes in Exec Login File
</commit_message>
<xml_diff>
--- a/GlobalDatafiles/TestData.xlsx
+++ b/GlobalDatafiles/TestData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -52,61 +52,397 @@
     <t>CreateStudentTags</t>
   </si>
   <si>
+    <t>DataProviderWithExcel</t>
+  </si>
+  <si>
+    <t>RandomFirstName</t>
+  </si>
+  <si>
+    <t>RandomLastName</t>
+  </si>
+  <si>
+    <t>autoqa</t>
+  </si>
+  <si>
+    <t>Test12345</t>
+  </si>
+  <si>
+    <t>QA - org</t>
+  </si>
+  <si>
+    <t>QA Program - 9th April</t>
+  </si>
+  <si>
+    <t>Enrolled</t>
+  </si>
+  <si>
+    <t>Section QA</t>
+  </si>
+  <si>
+    <t>Team QA</t>
+  </si>
+  <si>
     <t>Written Feedback</t>
-  </si>
-  <si>
-    <t>Team QA</t>
-  </si>
-  <si>
-    <t>Section QA</t>
-  </si>
-  <si>
-    <t>Potential</t>
-  </si>
-  <si>
-    <t>QA - org</t>
-  </si>
-  <si>
-    <t>RandomEmail</t>
-  </si>
-  <si>
-    <t>RandomLastName</t>
-  </si>
-  <si>
-    <t>RandomFirstName</t>
-  </si>
-  <si>
-    <t>DataProviderWithExcel</t>
-  </si>
-  <si>
-    <t>QA Program - 9th April</t>
-  </si>
-  <si>
-    <t>Test12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -114,24 +450,315 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
@@ -142,9 +769,7 @@
         <i val="0"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
@@ -157,9 +782,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -208,7 +830,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,7 +865,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,35 +1068,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="22.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="29.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="25.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="28.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="33.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="34.8571428571429" customWidth="1"/>
     <col min="11" max="11" width="33" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,45 +1134,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="autoqa"/>
+  </hyperlinks>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>